<commit_message>
add prices to items
</commit_message>
<xml_diff>
--- a/items.xlsx
+++ b/items.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
   <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+  <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\HP 840 G5\Documents\gitpractice\television\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\DELL\Documents\television\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
   <si>
     <t>S/N</t>
   </si>
@@ -60,12 +60,18 @@
   </si>
   <si>
     <t>Generator</t>
+  </si>
+  <si>
+    <t>Price</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$₦-470]#,##0.00"/>
+  </numFmts>
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -95,8 +101,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -377,10 +384,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+  <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+      <selection activeCell="J4" sqref="J4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -388,95 +395,129 @@
     <col min="2" max="2" width="11.90625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2">
         <v>1</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3">
         <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C3" s="1">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4">
         <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C4" s="1">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5">
         <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C5" s="1">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6">
         <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C6" s="1">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7">
         <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C7" s="1">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8">
         <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C8" s="1">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9">
         <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C9" s="1">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10">
         <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="C10" s="1">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11">
         <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>11</v>
       </c>
+      <c r="C11" s="1">
+        <v>10</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>